<commit_message>
Multiple custom layers options
</commit_message>
<xml_diff>
--- a/tests/fixtures/upload_table_sample.xlsx
+++ b/tests/fixtures/upload_table_sample.xlsx
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>COMUNE</t>
+          <t>Random_value_1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Random_value</t>
+          <t>Random_value_2</t>
         </is>
       </c>
     </row>
@@ -454,78 +454,62 @@
       <c r="A2" t="n">
         <v>21110</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Vandoies</t>
-        </is>
+      <c r="B2" t="n">
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>17214</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>15146</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Milano</t>
-        </is>
+      <c r="B3" t="n">
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>12784</v>
+        <v>568</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>16065</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Castro</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>42348</v>
-      </c>
+      <c r="B4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>58091</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Roma</t>
-        </is>
+      <c r="B5" t="n">
+        <v>7</v>
       </c>
       <c r="C5" t="n">
-        <v>4255</v>
+        <v>792</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>63049</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Napoli</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>26329</v>
+        <v>595</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>75096</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Castro</t>
-        </is>
+      <c r="B7" t="n">
+        <v>7</v>
       </c>
       <c r="C7" t="n">
-        <v>6782</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>